<commit_message>
Updated WP43 VANGLE update, Ben, 41d0055, 68904f2
</commit_message>
<xml_diff>
--- a/src/index spreadsheet/DM42 key template.xlsx
+++ b/src/index spreadsheet/DM42 key template.xlsx
@@ -1,18 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11009"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacomostert/wp43s/src/index spreadsheet/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580C2061-FFAF-3F48-AB51-6EC54F37BCDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="19020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -21,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="271">
   <si>
     <t>primary</t>
   </si>
@@ -831,12 +845,15 @@
   </si>
   <si>
     <t>-MNU_BASE</t>
+  </si>
+  <si>
+    <t>ITM_ARG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -967,6 +984,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1291,14 +1316,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
@@ -1312,7 +1337,7 @@
     <col min="10" max="10" width="108.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>178</v>
       </c>
@@ -1341,7 +1366,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -1373,7 +1398,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>140</v>
       </c>
@@ -1405,7 +1430,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -1437,7 +1462,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>142</v>
       </c>
@@ -1469,7 +1494,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -1501,7 +1526,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>145</v>
       </c>
@@ -1533,7 +1558,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>146</v>
       </c>
@@ -1565,7 +1590,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>147</v>
       </c>
@@ -1597,7 +1622,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>148</v>
       </c>
@@ -1608,7 +1633,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>58</v>
+        <v>270</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>10</v>
@@ -1629,7 +1654,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>150</v>
       </c>
@@ -1661,7 +1686,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>151</v>
       </c>
@@ -1693,7 +1718,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>152</v>
       </c>
@@ -1725,7 +1750,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>153</v>
       </c>
@@ -1757,7 +1782,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -1789,7 +1814,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>155</v>
       </c>
@@ -1821,7 +1846,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>156</v>
       </c>
@@ -1853,7 +1878,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>157</v>
       </c>
@@ -1885,7 +1910,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>158</v>
       </c>
@@ -1917,7 +1942,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>159</v>
       </c>
@@ -1949,7 +1974,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>160</v>
       </c>
@@ -1981,7 +2006,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>161</v>
       </c>
@@ -2013,7 +2038,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>162</v>
       </c>
@@ -2045,7 +2070,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>163</v>
       </c>
@@ -2077,7 +2102,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>164</v>
       </c>
@@ -2109,7 +2134,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>165</v>
       </c>
@@ -2141,7 +2166,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>166</v>
       </c>
@@ -2173,7 +2198,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>167</v>
       </c>
@@ -2205,7 +2230,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>168</v>
       </c>
@@ -2237,7 +2262,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>169</v>
       </c>
@@ -2269,7 +2294,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>170</v>
       </c>
@@ -2301,7 +2326,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>171</v>
       </c>
@@ -2333,7 +2358,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>172</v>
       </c>
@@ -2365,7 +2390,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>173</v>
       </c>
@@ -2397,7 +2422,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>174</v>
       </c>
@@ -2429,7 +2454,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>175</v>
       </c>
@@ -2461,7 +2486,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>176</v>
       </c>
@@ -2493,7 +2518,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>177</v>
       </c>
@@ -2537,14 +2562,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I38" sqref="B2:I38"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.5" customWidth="1"/>
@@ -2557,7 +2582,7 @@
     <col min="9" max="9" width="31.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" t="str">
         <f>Sheet1!B1</f>
         <v>primary</v>
@@ -2591,7 +2616,7 @@
         <v>primaryTam</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2628,7 +2653,7 @@
         <v xml:space="preserve">kbd_usr[0].primaryTam=ITM_ST_A; </v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2665,7 +2690,7 @@
         <v xml:space="preserve">kbd_usr[1].primaryTam=ITM_ST_B; </v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2702,7 +2727,7 @@
         <v xml:space="preserve">kbd_usr[2].primaryTam=ITM_ST_C; </v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2739,7 +2764,7 @@
         <v xml:space="preserve">kbd_usr[3].primaryTam=ITM_ST_D; </v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2776,7 +2801,7 @@
         <v xml:space="preserve">kbd_usr[4].primaryTam=ITM_NULL; </v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2813,7 +2838,7 @@
         <v xml:space="preserve">kbd_usr[5].primaryTam=CHR_alpha; </v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2850,7 +2875,7 @@
         <v xml:space="preserve">kbd_usr[6].primaryTam=ITM_NULL; </v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2887,7 +2912,7 @@
         <v xml:space="preserve">kbd_usr[7].primaryTam=ITM_HEX; </v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2901,7 +2926,7 @@
       </c>
       <c r="D10" t="str">
         <f>"kbd_usr["&amp;$A10&amp;"]."&amp;D$1&amp;"="&amp;Sheet1!D11&amp;"; "</f>
-        <v xml:space="preserve">kbd_usr[8].gShifted=ITM_ANGLE; </v>
+        <v xml:space="preserve">kbd_usr[8].gShifted=ITM_ARG; </v>
       </c>
       <c r="E10" t="str">
         <f>"kbd_usr["&amp;$A10&amp;"]."&amp;E$1&amp;"="&amp;Sheet1!E11&amp;"; "</f>
@@ -2924,7 +2949,7 @@
         <v xml:space="preserve">kbd_usr[8].primaryTam=ITM_REGI; </v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2961,7 +2986,7 @@
         <v xml:space="preserve">kbd_usr[9].primaryTam=ITM_REGJ; </v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2998,7 +3023,7 @@
         <v xml:space="preserve">kbd_usr[10].primaryTam=ITM_REGK; </v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3035,7 +3060,7 @@
         <v xml:space="preserve">kbd_usr[11].primaryTam=ITM_REGL; </v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3072,7 +3097,7 @@
         <v xml:space="preserve">kbd_usr[12].primaryTam=ITM_ENTER; </v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3109,7 +3134,7 @@
         <v xml:space="preserve">kbd_usr[13].primaryTam=ITM_NULL; </v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3146,7 +3171,7 @@
         <v xml:space="preserve">kbd_usr[14].primaryTam=ITM_NULL; </v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3183,7 +3208,7 @@
         <v xml:space="preserve">kbd_usr[15].primaryTam=ITM_NULL; </v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3220,7 +3245,7 @@
         <v xml:space="preserve">kbd_usr[16].primaryTam=KEY_BACKSPACE}; </v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3257,7 +3282,7 @@
         <v xml:space="preserve">kbd_usr[17].primaryTam=KEY_UP1; </v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -3294,7 +3319,7 @@
         <v xml:space="preserve">kbd_usr[18].primaryTam=CHR_7; </v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3331,7 +3356,7 @@
         <v xml:space="preserve">kbd_usr[19].primaryTam=CHR_8; </v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3368,7 +3393,7 @@
         <v xml:space="preserve">kbd_usr[20].primaryTam=CHR_9; </v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -3405,7 +3430,7 @@
         <v xml:space="preserve">kbd_usr[21].primaryTam=ITM_DIV; </v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3442,7 +3467,7 @@
         <v xml:space="preserve">kbd_usr[22].primaryTam=KEY_DOWN1; </v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3479,7 +3504,7 @@
         <v xml:space="preserve">kbd_usr[23].primaryTam=CHR_4; </v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3516,7 +3541,7 @@
         <v xml:space="preserve">kbd_usr[24].primaryTam=CHR_5; </v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3553,7 +3578,7 @@
         <v xml:space="preserve">kbd_usr[25].primaryTam=CHR_6; </v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3590,7 +3615,7 @@
         <v xml:space="preserve">kbd_usr[26].primaryTam=ITM_MULT; </v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3627,7 +3652,7 @@
         <v xml:space="preserve">kbd_usr[27].primaryTam=KEY_fg; </v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -3664,7 +3689,7 @@
         <v xml:space="preserve">kbd_usr[28].primaryTam=CHR_1; </v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3701,7 +3726,7 @@
         <v xml:space="preserve">kbd_usr[29].primaryTam=CHR_2; </v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -3738,7 +3763,7 @@
         <v xml:space="preserve">kbd_usr[30].primaryTam=CHR_3; </v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -3775,7 +3800,7 @@
         <v xml:space="preserve">kbd_usr[31].primaryTam=ITM_SUB; </v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -3812,7 +3837,7 @@
         <v xml:space="preserve">kbd_usr[32].primaryTam=KEY_EXIT1; </v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -3849,7 +3874,7 @@
         <v xml:space="preserve">kbd_usr[33].primaryTam=CHR_0; </v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -3886,7 +3911,7 @@
         <v xml:space="preserve">kbd_usr[34].primaryTam=CHR_PERIOD; </v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -3923,7 +3948,7 @@
         <v xml:space="preserve">kbd_usr[35].primaryTam=ITM_NULL; </v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -3972,14 +3997,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AO44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:J43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
@@ -4012,7 +4037,7 @@
     <col min="41" max="41" width="8.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:41">
+    <row r="1" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
         <v>217</v>
@@ -4041,7 +4066,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="2:41">
+    <row r="2" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -4070,7 +4095,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="2:41">
+    <row r="3" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>37</v>
@@ -4099,7 +4124,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="2:41">
+    <row r="4" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>27</v>
@@ -4194,7 +4219,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="2:41">
+    <row r="5" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
         <v>25</v>
@@ -4223,7 +4248,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="2:41">
+    <row r="6" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
         <v>95</v>
@@ -4252,7 +4277,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="8" spans="2:41">
+    <row r="8" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
         <v>42</v>
@@ -4281,7 +4306,7 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="2:41">
+    <row r="9" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>45</v>
@@ -4310,7 +4335,7 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="2:41">
+    <row r="10" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
         <v>51</v>
@@ -4381,7 +4406,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="11" spans="2:41">
+    <row r="11" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
         <v>249</v>
@@ -4410,7 +4435,7 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="2:41">
+    <row r="12" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>253</v>
@@ -4439,7 +4464,7 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="2:41">
+    <row r="13" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
         <v>255</v>
@@ -4468,7 +4493,7 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="15" spans="2:41">
+    <row r="15" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
         <v>63</v>
@@ -4497,7 +4522,7 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="2:41">
+    <row r="16" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>64</v>
@@ -4526,7 +4551,7 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="2:12">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
         <v>69</v>
@@ -4555,7 +4580,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
         <v>75</v>
@@ -4584,7 +4609,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="2:12">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
         <v>80</v>
@@ -4612,7 +4637,7 @@
       </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
         <v>213</v>
@@ -4641,7 +4666,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
         <v>86</v>
@@ -4670,7 +4695,7 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="2:12">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
         <v>89</v>
@@ -4699,7 +4724,7 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="2:12">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
         <v>92</v>
@@ -4728,7 +4753,7 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="2:12">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
         <v>82</v>
@@ -4757,7 +4782,7 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="27" spans="2:12">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
         <v>214</v>
@@ -4786,7 +4811,7 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="2:12">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
         <v>102</v>
@@ -4815,7 +4840,7 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="2:12">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
         <v>105</v>
@@ -4844,7 +4869,7 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="2:12">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
         <v>108</v>
@@ -4873,7 +4898,7 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
-    <row r="31" spans="2:12">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
         <v>98</v>
@@ -4902,7 +4927,7 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
         <v>263</v>
@@ -4931,7 +4956,7 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>115</v>
@@ -4960,7 +4985,7 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
         <v>118</v>
@@ -4989,7 +5014,7 @@
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
         <v>121</v>
@@ -5018,7 +5043,7 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
         <v>112</v>
@@ -5047,7 +5072,7 @@
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
         <v>212</v>
@@ -5076,7 +5101,7 @@
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
         <v>130</v>
@@ -5105,7 +5130,7 @@
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
         <v>132</v>
@@ -5134,7 +5159,7 @@
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
         <v>134</v>
@@ -5163,7 +5188,7 @@
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
         <v>126</v>
@@ -5192,7 +5217,7 @@
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>

</xml_diff>